<commit_message>
Segunda version de GIT
</commit_message>
<xml_diff>
--- a/MPage/MPage.xlsx
+++ b/MPage/MPage.xlsx
@@ -98,7 +98,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="215">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -740,6 +740,9 @@
   </si>
   <si>
     <t>Costo</t>
+  </si>
+  <si>
+    <t>Cambio nuevo para git</t>
   </si>
 </sst>
 </file>
@@ -1426,7 +1429,7 @@
   <dimension ref="A1:BP46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="L12" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="S28" sqref="S28"/>
+      <selection activeCell="Q31" sqref="Q31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3240,6 +3243,9 @@
       <c r="D30" s="41">
         <f>C30/45</f>
         <v>3.3333333333333335</v>
+      </c>
+      <c r="Q30" s="19" t="s">
+        <v>214</v>
       </c>
       <c r="AO30" s="19"/>
       <c r="AP30" s="19"/>

</xml_diff>